<commit_message>
Lot of changes. Mainly adding the importer and using it and using freemarker template for the web module
</commit_message>
<xml_diff>
--- a/importer/src/test/resources/testdata/extract_only_names.xlsx
+++ b/importer/src/test/resources/testdata/extract_only_names.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -29,13 +29,40 @@
     <t>location</t>
   </si>
   <si>
-    <t>kola</t>
+    <t>Kola</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>kola means</t>
+  </si>
+  <si>
+    <t>oyo</t>
   </si>
   <si>
     <t>koko</t>
   </si>
   <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>koko means</t>
+  </si>
+  <si>
+    <t>lagos</t>
+  </si>
+  <si>
     <t>Dadepo</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>dadepo means</t>
+  </si>
+  <si>
+    <t>ife</t>
   </si>
 </sst>
 </file>
@@ -271,7 +298,7 @@
   <dimension ref="1:340"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -303,15 +330,42 @@
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>